<commit_message>
Auto commit: 2025-08-22 20:26:30
</commit_message>
<xml_diff>
--- a/888.xlsx
+++ b/888.xlsx
@@ -1,179 +1,205 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="27945" windowHeight="12375" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView windowWidth="19200" windowHeight="6880"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="144525" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+  <si>
+    <t>thhhdhdhdhddhd</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="20">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -473,156 +499,156 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,74 +704,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -997,58 +960,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="E9:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="9" spans="5:5">
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5">
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>